<commit_message>
Ya funciona al 100 el primer for
</commit_message>
<xml_diff>
--- a/marco.xlsx
+++ b/marco.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="main" sheetId="3" r:id="rId1"/>
     <sheet name="bucket" sheetId="1" r:id="rId2"/>
+    <sheet name="getMax" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="41">
   <si>
     <t>address</t>
   </si>
@@ -143,12 +144,6 @@
   </si>
   <si>
     <t>max</t>
-  </si>
-  <si>
-    <t>bucket</t>
-  </si>
-  <si>
-    <t>a2</t>
   </si>
 </sst>
 </file>
@@ -236,106 +231,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="18">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFCDCD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFCDCD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFCDCD"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -354,32 +255,53 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFCDCD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
       <bottom style="thin">
         <color rgb="FFFFCDCD"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FFFFCC99"/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFFFCC99"/>
+        <color rgb="FFFFCDCD"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color theme="1"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
@@ -397,201 +319,6 @@
         <color indexed="64"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFCDCD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFFFCDCD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFFFCDCD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFFFCC99"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFCC99"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFCC99"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFCC99"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFCC99FF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FFCC99FF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCC99FF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFCC99FF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCC99FF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFCC99FF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCC99FF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFCC99FF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFCC99FF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFCDCD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFCDCD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color theme="1"/>
-      </right>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFCDCD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFCDCD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color theme="1"/>
       </right>
       <top style="thin">
@@ -767,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -786,12 +513,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -804,76 +531,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -885,28 +567,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -917,9 +587,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC99FF"/>
+      <color rgb="FFFFCC99"/>
       <color rgb="FFFFCDCD"/>
-      <color rgb="FFFFCC99"/>
-      <color rgb="FFCC99FF"/>
       <color rgb="FFFF6699"/>
       <color rgb="FFFFA7A7"/>
       <color rgb="FFFF9966"/>
@@ -1218,16 +888,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
       <c r="G1" s="16" t="s">
         <v>35</v>
       </c>
@@ -1268,12 +938,12 @@
       <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="26"/>
       <c r="G3" s="18">
         <v>0</v>
       </c>
@@ -1289,12 +959,12 @@
       <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="29"/>
       <c r="G4" s="18">
         <v>-4</v>
       </c>
@@ -1310,10 +980,10 @@
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="29"/>
       <c r="G5" s="18">
         <v>-8</v>
       </c>
@@ -1329,10 +999,10 @@
       <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="31"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="18">
         <v>-12</v>
       </c>
@@ -1385,10 +1055,10 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="K9" s="20" t="s">
+      <c r="K9" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="21"/>
+      <c r="L9" s="22"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -1677,7 +1347,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,27 +1364,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
       <c r="G1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1739,17 +1409,17 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>2147483632</v>
+        <v>2147483616</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="46"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
       <c r="G3" s="17">
         <v>0</v>
       </c>
@@ -1757,20 +1427,21 @@
         <v>44</v>
       </c>
       <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
-        <v>2147483628</v>
+        <v>2147483612</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="48"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
       <c r="G4" s="17">
         <v>-4</v>
       </c>
@@ -1779,17 +1450,17 @@
       </c>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
-        <v>2147483624</v>
+        <v>2147483608</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="48"/>
+        <v>9</v>
+      </c>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
       <c r="G5" s="17">
         <v>-8</v>
       </c>
@@ -1797,18 +1468,22 @@
         <v>36</v>
       </c>
       <c r="I5" s="5"/>
+      <c r="K5" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="22"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>2147483620</v>
+        <v>2147483604</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="54"/>
+        <v>10</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="17">
         <v>-12</v>
       </c>
@@ -1816,20 +1491,24 @@
         <v>32</v>
       </c>
       <c r="I6" s="5"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>2147483616</v>
+        <v>2147483600</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="51"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
       <c r="G7" s="17">
         <v>-16</v>
       </c>
@@ -1837,21 +1516,24 @@
         <v>28</v>
       </c>
       <c r="I7" s="5"/>
-      <c r="K7" s="7"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="13" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
-        <v>2147483612</v>
+        <v>2147483596</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="37"/>
+        <v>12</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
       <c r="G8" s="17">
         <v>-20</v>
       </c>
@@ -1859,20 +1541,24 @@
         <v>24</v>
       </c>
       <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K8" s="14"/>
+      <c r="L8" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>2147483608</v>
+        <v>2147483592</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="37"/>
+        <v>13</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="17">
         <v>-24</v>
       </c>
@@ -1880,24 +1566,20 @@
         <v>20</v>
       </c>
       <c r="I9" s="5"/>
-      <c r="K9" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="L9" s="21"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>2147483604</v>
+        <v>2147483588</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="51"/>
+        <v>14</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
       <c r="G10" s="17">
         <v>-28</v>
       </c>
@@ -1905,24 +1587,20 @@
         <v>16</v>
       </c>
       <c r="I10" s="5"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="11" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>2147483600</v>
+        <v>2147483584</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="40"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
       <c r="G11" s="17">
         <v>-32</v>
       </c>
@@ -1930,24 +1608,21 @@
         <v>12</v>
       </c>
       <c r="I11" s="5"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>2147483596</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="41" t="s">
+        <v>2147483580</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="43"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
       <c r="G12" s="17">
         <v>-36</v>
       </c>
@@ -1955,24 +1630,18 @@
         <v>8</v>
       </c>
       <c r="I12" s="5"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="15" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>2147483592</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="40"/>
+        <v>2147483576</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
       <c r="G13" s="17">
         <v>-40</v>
       </c>
@@ -1980,20 +1649,18 @@
         <v>4</v>
       </c>
       <c r="I13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>2147483588</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="34"/>
+        <v>2147483572</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
       <c r="G14" s="17">
         <v>-44</v>
       </c>
@@ -2004,10 +1671,10 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>2147483584</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>15</v>
+        <v>2147483568</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -2016,14 +1683,13 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>2147483580</v>
+        <v>2147483564</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -2035,10 +1701,10 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>2147483576</v>
+        <v>2147483560</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -2050,10 +1716,10 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>2147483572</v>
+        <v>2147483556</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2065,10 +1731,10 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>2147483568</v>
+        <v>2147483552</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -2080,10 +1746,10 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>2147483564</v>
+        <v>2147483548</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -2095,10 +1761,10 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>2147483560</v>
+        <v>2147483544</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -2110,10 +1776,10 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>2147483556</v>
+        <v>2147483540</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -2203,6 +1869,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C3:F3"/>
@@ -2212,14 +1884,470 @@
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L22"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="4.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="41.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2147483616</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="17">
+        <v>0</v>
+      </c>
+      <c r="H3" s="17">
+        <v>44</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>2147483612</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="17">
+        <v>-4</v>
+      </c>
+      <c r="H4" s="17">
+        <v>40</v>
+      </c>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>2147483608</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="17">
+        <v>-8</v>
+      </c>
+      <c r="H5" s="17">
+        <v>36</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="K5" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="22"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>2147483604</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="17">
+        <v>-12</v>
+      </c>
+      <c r="H6" s="17">
+        <v>32</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>2147483600</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="17">
+        <v>-16</v>
+      </c>
+      <c r="H7" s="17">
+        <v>28</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>2147483596</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="17">
+        <v>-20</v>
+      </c>
+      <c r="H8" s="17">
+        <v>24</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>2147483592</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="17">
+        <v>-24</v>
+      </c>
+      <c r="H9" s="17">
+        <v>20</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>2147483588</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="17">
+        <v>-28</v>
+      </c>
+      <c r="H10" s="17">
+        <v>16</v>
+      </c>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>2147483584</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="17">
+        <v>-32</v>
+      </c>
+      <c r="H11" s="17">
+        <v>12</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>2147483580</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="17">
+        <v>-36</v>
+      </c>
+      <c r="H12" s="17">
+        <v>8</v>
+      </c>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>2147483576</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="17">
+        <v>-40</v>
+      </c>
+      <c r="H13" s="17">
+        <v>4</v>
+      </c>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>2147483572</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="17">
+        <v>-44</v>
+      </c>
+      <c r="H14" s="17">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>2147483568</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>2147483564</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>2147483560</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>2147483556</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>2147483552</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>2147483548</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>2147483544</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>2147483540</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>